<commit_message>
Add fans and other small electronic bits
Signed-off-by: Misha Turnbull <mishaturnbull@gmail.com>
</commit_message>
<xml_diff>
--- a/Laptop_build.xlsx
+++ b/Laptop_build.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
   <si>
     <t xml:space="preserve">Part</t>
   </si>
@@ -249,6 +249,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.amazon.com/Inline-Coupler-AVACON-Ethernet-Female/dp/B07DWPW5MJ/ref=sr_1_5?keywords=gigabit+ethernet+coupler&amp;qid=1562638098&amp;s=gateway&amp;sr=8-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooling fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mini 5V cooling fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.adafruit.com/product/3368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMP36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/analog-devices-inc/TMP36GT9Z/820404</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -518,8 +536,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K24" headerRowCount="1" totalsRowCount="1" totalsRowShown="1">
-  <autoFilter ref="A1:K24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K26" headerRowCount="1" totalsRowCount="1" totalsRowShown="1">
+  <autoFilter ref="A1:K26"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Part"/>
     <tableColumn id="2" name="Name"/>
@@ -541,13 +559,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.79"/>
@@ -1385,37 +1403,113 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="0"/>
+      <c r="B24" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>3.5</v>
+      </c>
       <c r="E24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" s="4" t="n">
+        <f aca="false">Table1[[#This Row],[Price per]]*Table1[[#This Row],[Quantity]]</f>
+        <v>10.5</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <f aca="false">Table1[[#This Row],[Power draw (A)]]*Table1[[#This Row],[Power supply (V)]]*Table1[[#This Row],[Quantity]]</f>
+        <v>3</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <f aca="false">Table1[[#This Row],[Weight (g)]]*Table1[[#This Row],[Quantity]]</f>
+        <v>18.6</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F25" s="4" t="n">
+        <f aca="false">Table1[[#This Row],[Price per]]*Table1[[#This Row],[Quantity]]</f>
+        <v>5.92</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <f aca="false">Table1[[#This Row],[Power draw (A)]]*Table1[[#This Row],[Power supply (V)]]*Table1[[#This Row],[Quantity]]</f>
+        <v>0.002</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <f aca="false">Table1[[#This Row],[Weight (g)]]*Table1[[#This Row],[Quantity]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Quantity])</f>
-        <v>24</v>
-      </c>
-      <c r="F24" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="F26" s="4" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Price total])</f>
-        <v>1313.47</v>
-      </c>
-      <c r="G24" s="0" t="n">
+        <v>1329.89</v>
+      </c>
+      <c r="G26" s="0" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Power draw (A)])</f>
-        <v>13.18293</v>
-      </c>
-      <c r="H24" s="0" t="n">
+        <v>13.38303</v>
+      </c>
+      <c r="H26" s="0" t="n">
         <f aca="false">SUBTOTAL(104,Table1[Power supply (V)])</f>
         <v>19</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="I26" s="0" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Watt total])</f>
-        <v>87.06749</v>
-      </c>
-      <c r="K24" s="0" t="n">
+        <v>90.06949</v>
+      </c>
+      <c r="K26" s="0" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Weight total])</f>
-        <v>3819.09</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>3837.69</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="0"/>
+      <c r="F27" s="4"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://www.udoo.org/udoo-bolt/"/>
@@ -1459,14 +1553,14 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1483,13 +1577,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1497,43 +1591,43 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>4</v>
@@ -1541,10 +1635,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1.6</v>

</xml_diff>

<commit_message>
Update link for ethernet port that went unavail
Signed-off-by: Misha Turnbull <mishaturnbull@gmail.com>
</commit_message>
<xml_diff>
--- a/Laptop_build.xlsx
+++ b/Laptop_build.xlsx
@@ -248,7 +248,7 @@
     <t xml:space="preserve">RJ45 coupler 10Gb</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.amazon.com/Inline-Coupler-AVACON-Ethernet-Female/dp/B07DWPW5MJ/ref=sr_1_5?keywords=gigabit+ethernet+coupler&amp;qid=1562638098&amp;s=gateway&amp;sr=8-5</t>
+    <t xml:space="preserve">https://www.amazon.com/Haitronic-ethernet-Connector-Ethernet-Extender/dp/B06XPZBRJ2/136-8664393-2449817?psc=1</t>
   </si>
   <si>
     <t xml:space="preserve">Cooling fan</t>
@@ -561,11 +561,11 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.79"/>
@@ -1365,7 +1365,7 @@
         <v>18.14</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>73</v>
       </c>
@@ -1527,7 +1527,6 @@
     <hyperlink ref="C19" r:id="rId13" display="https://www.amazon.com/Besgoods-Charging-Braided-Compatible-Nintendo/dp/B07H24V7YJ/ref=sr_1_6?keywords=usb-c+cable+2ft&amp;qid=1562636637&amp;s=pc&amp;sr=1-6"/>
     <hyperlink ref="C21" r:id="rId14" display="https://www.amazon.com/RIITOP-Extender-Extension-Nintendo-Macbook/dp/B07NSXGM7F/ref=sxin_2_ac_d_pm?keywords=usb%2Bc%2Bextension%2Bcable&amp;pd_rd_i=B01LI2X4ME&amp;pd_rd_r=ecef4ce7-409b-40a0-9a92-4a28c759c2de&amp;pd_rd_w=wUSD8&amp;pd_rd_wg=FpYjh&amp;pf_rd_p=64aaff2e-3b89-4fee-a107-2469ecbc5733&amp;pf_rd_r=T7G96XX8V6BS81KAA74N&amp;qid=1562637699&amp;s=aht&amp;th=1"/>
     <hyperlink ref="C22" r:id="rId15" display="https://www.amazon.com/Monoprice-Flexboot-Ethernet-Patch-Cable/dp/B00AJHCMG4/ref=sr_1_9?keywords=rj45+patch+cable+1ft&amp;qid=1562637988&amp;s=gateway&amp;sr=8-9"/>
-    <hyperlink ref="C23" r:id="rId16" display="https://www.amazon.com/Inline-Coupler-AVACON-Ethernet-Female/dp/B07DWPW5MJ/ref=sr_1_5?keywords=gigabit+ethernet+coupler&amp;qid=1562638098&amp;s=gateway&amp;sr=8-5"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1537,7 +1536,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1549,11 +1548,11 @@
   </sheetPr>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.95"/>
   </cols>

</xml_diff>

<commit_message>
Add numpad power draw
.25 AMPs?? WTF??

Signed-off-by: Misha Turnbull <mishaturnbull@gmail.com>
</commit_message>
<xml_diff>
--- a/Laptop_build.xlsx
+++ b/Laptop_build.xlsx
@@ -561,11 +561,11 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.79"/>
@@ -1131,12 +1131,15 @@
         <f aca="false">Table1[[#This Row],[Price per]]*Table1[[#This Row],[Quantity]]</f>
         <v>7.99</v>
       </c>
+      <c r="G16" s="0" t="n">
+        <v>0.25</v>
+      </c>
       <c r="H16" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I16" s="0" t="n">
         <f aca="false">Table1[[#This Row],[Power draw (A)]]*Table1[[#This Row],[Power supply (V)]]*Table1[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>120</v>
@@ -1491,7 +1494,7 @@
       </c>
       <c r="G26" s="0" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Power draw (A)])</f>
-        <v>13.38303</v>
+        <v>13.63303</v>
       </c>
       <c r="H26" s="0" t="n">
         <f aca="false">SUBTOTAL(104,Table1[Power supply (V)])</f>
@@ -1499,7 +1502,7 @@
       </c>
       <c r="I26" s="0" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Watt total])</f>
-        <v>90.06949</v>
+        <v>91.31949</v>
       </c>
       <c r="K26" s="0" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Weight total])</f>
@@ -1548,11 +1551,11 @@
   </sheetPr>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.95"/>
   </cols>

</xml_diff>

<commit_message>
A programmer's attempt at a battery calculator
Signed-off-by: Misha Turnbull <mishaturnbull@gmail.com>
</commit_message>
<xml_diff>
--- a/Laptop_build.xlsx
+++ b/Laptop_build.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Cooling" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="BatteryReqs" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="120">
   <si>
     <t xml:space="preserve">Part</t>
   </si>
@@ -312,17 +313,87 @@
   </si>
   <si>
     <t xml:space="preserve">mineral oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Per Battery Pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N. Battery Packs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power system available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life expectancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N. 18650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Series</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Wh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power draw (from Parts sheet), W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V/cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total mAh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to death (h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mAh/cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available power (W)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mAh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C rating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only input on this color!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WARNING: THIS SPREADSHEET IS LIKELY WRONG.  I am not an electrical engineer, and it has not (yet) been looked over by one!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -361,21 +432,91 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDBB6"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF38"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -427,7 +568,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -454,6 +595,82 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -472,18 +689,68 @@
     <cellStyle name="Pivot Table Value" xfId="26"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="1"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFFF38"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -497,7 +764,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0563C1"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -513,7 +780,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFDBB6"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -526,7 +793,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -561,11 +828,11 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.79"/>
@@ -1555,7 +1822,7 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.95"/>
   </cols>
@@ -1658,4 +1925,281 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O24"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.9"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="I1" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="L1" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="9" t="n">
+        <f aca="false">B6*B5</f>
+        <v>8</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="10" t="n">
+        <f aca="false">B3*B5</f>
+        <v>14.4</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" s="12" t="n">
+        <f aca="false">J3*J4/1000</f>
+        <v>144</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="12" t="n">
+        <f aca="false">Parts!I26</f>
+        <v>91.31949</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="14" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="10" t="n">
+        <f aca="false">B4*B7/1000*B6</f>
+        <v>5</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="12" t="n">
+        <f aca="false">G3*D5</f>
+        <v>10000</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="12" t="n">
+        <f aca="false">J2/O2</f>
+        <v>1.57688134263562</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="14" t="n">
+        <v>2500</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="10" t="n">
+        <f aca="false">D3*D2</f>
+        <v>72</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J4" s="12" t="n">
+        <f aca="false">D2*G2</f>
+        <v>14.4</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="18" t="n">
+        <f aca="false">J5*J4</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="10" t="n">
+        <f aca="false">B6*B4</f>
+        <v>5000</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="18" t="n">
+        <f aca="false">G3*D3</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="10" t="n">
+        <f aca="false">D5*D2/1000</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D21" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="F12:G15"/>
+    <mergeCell ref="D21:G24"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="cellIs" priority="2" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4">
+    <cfRule type="cellIs" priority="3" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>BatteryReqs!$O$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4">
+    <cfRule type="cellIs" priority="4" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>BatteryReqs!$O$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" priority="5" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Not sure what changed :(
Signed-off-by: Misha Turnbull <mishaturnbull@gmail.com>
</commit_message>
<xml_diff>
--- a/Laptop_build.xlsx
+++ b/Laptop_build.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="125">
   <si>
     <t xml:space="preserve">Part</t>
   </si>
@@ -378,10 +378,25 @@
     <t xml:space="preserve">C rating</t>
   </si>
   <si>
+    <t xml:space="preserve">Watt-amp avail &amp; draw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rail voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avail (A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draw (A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draw (W)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Only input on this color!</t>
   </si>
   <si>
-    <t xml:space="preserve">WARNING: THIS SPREADSHEET IS LIKELY WRONG.  I am not an electrical engineer, and it has not (yet) been looked over by one!</t>
+    <t xml:space="preserve">WARNING: THIS SPREADSHEET IS LIKELY WRONG.  I am not an electrical engineer, and it has not (yet) been looked over by one!  Some of the formulas are KNOWN TO BE INCORRECT!</t>
   </si>
 </sst>
 </file>
@@ -568,7 +583,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -617,10 +632,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -665,11 +676,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -829,10 +852,10 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.79"/>
@@ -1154,11 +1177,11 @@
         <v>0.00393</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="I9" s="0" t="n">
         <f aca="false">Table1[[#This Row],[Power draw (A)]]*Table1[[#This Row],[Power supply (V)]]*Table1[[#This Row],[Quantity]]</f>
-        <v>0.01179</v>
+        <v>0.012969</v>
       </c>
       <c r="K9" s="0" t="n">
         <f aca="false">Table1[[#This Row],[Weight (g)]]*Table1[[#This Row],[Quantity]]</f>
@@ -1214,11 +1237,11 @@
         <v>74.89</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="4" t="n">
         <f aca="false">Table1[[#This Row],[Price per]]*Table1[[#This Row],[Quantity]]</f>
-        <v>224.67</v>
+        <v>149.78</v>
       </c>
       <c r="I11" s="0" t="n">
         <f aca="false">Table1[[#This Row],[Power draw (A)]]*Table1[[#This Row],[Power supply (V)]]*Table1[[#This Row],[Quantity]]</f>
@@ -1229,7 +1252,7 @@
       </c>
       <c r="K11" s="0" t="n">
         <f aca="false">Table1[[#This Row],[Weight (g)]]*Table1[[#This Row],[Quantity]]</f>
-        <v>2259</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1753,11 +1776,11 @@
       <c r="D26" s="0"/>
       <c r="E26" s="0" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Quantity])</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F26" s="4" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Price total])</f>
-        <v>1329.89</v>
+        <v>1255</v>
       </c>
       <c r="G26" s="0" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Power draw (A)])</f>
@@ -1769,11 +1792,11 @@
       </c>
       <c r="I26" s="0" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Watt total])</f>
-        <v>91.31949</v>
+        <v>91.320669</v>
       </c>
       <c r="K26" s="0" t="n">
         <f aca="false">SUBTOTAL(109,Table1[Weight total])</f>
-        <v>3837.69</v>
+        <v>3084.69</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,7 +1845,7 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.95"/>
   </cols>
@@ -1935,10 +1958,10 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.9"/>
   </cols>
@@ -1978,7 +2001,7 @@
       </c>
       <c r="D2" s="10" t="n">
         <f aca="false">B3*B5</f>
-        <v>14.4</v>
+        <v>14</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>103</v>
@@ -1989,93 +2012,93 @@
       <c r="I2" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="12" t="n">
+      <c r="J2" s="10" t="n">
         <f aca="false">J3*J4/1000</f>
-        <v>144</v>
-      </c>
-      <c r="L2" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="12" t="n">
-        <f aca="false">Parts!I26</f>
-        <v>91.31949</v>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="10" t="n">
+        <f aca="false">SUM(L11:L13)</f>
+        <v>84.319169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="14" t="n">
-        <v>3.6</v>
+      <c r="B3" s="13" t="n">
+        <v>3.5</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>107</v>
       </c>
       <c r="D3" s="10" t="n">
         <f aca="false">B4*B7/1000*B6</f>
-        <v>5</v>
-      </c>
-      <c r="F3" s="15" t="s">
+        <v>5.5</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="16" t="n">
+      <c r="G3" s="15" t="n">
         <v>2</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="12" t="n">
+      <c r="J3" s="10" t="n">
         <f aca="false">G3*D5</f>
-        <v>10000</v>
-      </c>
-      <c r="L3" s="13" t="s">
+        <v>11000</v>
+      </c>
+      <c r="L3" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="12" t="n">
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="10" t="n">
         <f aca="false">J2/O2</f>
-        <v>1.57688134263562</v>
+        <v>1.82639371125681</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="14" t="n">
-        <v>2500</v>
+      <c r="B4" s="13" t="n">
+        <v>2750</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>112</v>
       </c>
       <c r="D4" s="10" t="n">
         <f aca="false">D3*D2</f>
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="J4" s="12" t="n">
+      <c r="J4" s="10" t="n">
         <f aca="false">D2*G2</f>
-        <v>14.4</v>
-      </c>
-      <c r="L4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="18" t="n">
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="17" t="n">
         <f aca="false">J5*J4</f>
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="14" t="n">
+      <c r="B5" s="13" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
@@ -2083,50 +2106,119 @@
       </c>
       <c r="D5" s="10" t="n">
         <f aca="false">B6*B4</f>
-        <v>5000</v>
-      </c>
-      <c r="I5" s="15" t="s">
+        <v>5500</v>
+      </c>
+      <c r="I5" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="J5" s="18" t="n">
+      <c r="J5" s="17" t="n">
         <f aca="false">G3*D3</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="19" t="n">
+      <c r="B6" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>116</v>
       </c>
       <c r="D6" s="10" t="n">
         <f aca="false">D5*D2/1000</f>
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I9" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I10" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="L10" s="23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="8" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <f aca="false">O4/I11</f>
+        <v>46.6666666666667</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">SUMIFS(Parts!G$2:G$25,Parts!H$2:H$25,I11)</f>
+        <v>1.73293</v>
+      </c>
+      <c r="L11" s="23" t="n">
+        <f aca="false">K11*I11</f>
+        <v>5.718669</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F12" s="24" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="G12" s="24"/>
+      <c r="I12" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <f aca="false">O4/I12</f>
+        <v>30.8</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <f aca="false">SUMIFS(Parts!G$2:G$25,Parts!H$2:H$25,I12)</f>
+        <v>3.7501</v>
+      </c>
+      <c r="L12" s="23" t="n">
+        <f aca="false">K12*I12</f>
+        <v>18.7505</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
+      <c r="I13" s="25" t="n">
+        <v>19</v>
+      </c>
+      <c r="J13" s="26" t="n">
+        <f aca="false">O4/I13</f>
+        <v>8.10526315789474</v>
+      </c>
+      <c r="K13" s="26" t="n">
+        <f aca="false">SUMIFS(Parts!G$2:G$25,Parts!H$2:H$25,I13)</f>
+        <v>3.15</v>
+      </c>
+      <c r="L13" s="17" t="n">
+        <f aca="false">K13*I13</f>
+        <v>59.85</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F14" s="24"/>
@@ -2137,33 +2229,33 @@
       <c r="G15" s="24"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D21" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
+      <c r="D21" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:J1"/>
@@ -2171,6 +2263,7 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L3:N3"/>
     <mergeCell ref="L4:N4"/>
+    <mergeCell ref="I9:L9"/>
     <mergeCell ref="F12:G15"/>
     <mergeCell ref="D21:G24"/>
   </mergeCells>

</xml_diff>